<commit_message>
Added two columns to the student data
</commit_message>
<xml_diff>
--- a/data/phd.xlsx
+++ b/data/phd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaitsev/Documents/Pharo/images/UMR SENS/pharo-local/iceberg/olekscode/umr-sens-presentation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30171FEF-9F5E-1645-A154-91B5EE587C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EAFCC0-E474-7F42-A0FB-056CF5295B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{F047E2A1-6D87-9F41-8491-8AF18799266C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="197">
   <si>
     <t>François</t>
   </si>
@@ -492,13 +492,155 @@
   <si>
     <t xml:space="preserve">H
 </t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Discipline</t>
+  </si>
+  <si>
+    <t>Social-Ecology</t>
+  </si>
+  <si>
+    <t>Antropology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antropology </t>
+  </si>
+  <si>
+    <t>Socio-Antropology</t>
+  </si>
+  <si>
+    <t>Antropology </t>
+  </si>
+  <si>
+    <t>Ethnology</t>
+  </si>
+  <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Rural Economics</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>Agronomy</t>
+  </si>
+  <si>
+    <t>Ethnoecology</t>
+  </si>
+  <si>
+    <t> Ethnoecology and Paleoecology </t>
+  </si>
+  <si>
+    <t>Antropology and Social Geography</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agronomy </t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Modeling</t>
+  </si>
+  <si>
+    <t>Computer science</t>
+  </si>
+  <si>
+    <t>Forests</t>
+  </si>
+  <si>
+    <t>Life Sciences</t>
+  </si>
+  <si>
+    <t>Economics and Agronomy</t>
+  </si>
+  <si>
+    <t>Environmental Sciences</t>
+  </si>
+  <si>
+    <t>Durable Development</t>
+  </si>
+  <si>
+    <t>Interdisciplinary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-40C]mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="dd\/mm\/yyyy"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -541,6 +683,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -559,13 +706,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -588,50 +736,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{C66EC5CE-FD8F-5842-BE76-36626479D022}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{D5FE63CF-FFBC-6F4F-8292-95760ED0D2E7}"/>
     <cellStyle name="Normal_Feuil1" xfId="2" xr:uid="{44FC2E6B-D61B-1349-84DA-48C69E802DFB}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -944,95 +1099,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20441DCD-30DD-2140-AD11-E091861272C1}">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="18" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="19" customWidth="1"/>
-    <col min="5" max="16" width="10.83203125" style="7"/>
+    <col min="3" max="4" width="10.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="7" customWidth="1"/>
+    <col min="6" max="17" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>0</v>
+      <c r="D2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="F2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="b">
         <v>0</v>
@@ -1050,30 +1208,33 @@
         <v>0</v>
       </c>
       <c r="N2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="2" t="b">
-        <v>0</v>
+      <c r="D3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="F3" s="2" t="b">
         <v>0</v>
@@ -1088,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="2" t="b">
         <v>0</v>
@@ -1100,33 +1261,36 @@
         <v>0</v>
       </c>
       <c r="N3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <v>1</v>
+      <c r="D4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="F4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>0</v>
@@ -1138,10 +1302,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2" t="b">
         <v>0</v>
@@ -1150,39 +1314,42 @@
         <v>0</v>
       </c>
       <c r="N4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="2" t="b">
-        <v>0</v>
+      <c r="D5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="F5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="b">
         <v>0</v>
@@ -1200,30 +1367,33 @@
         <v>0</v>
       </c>
       <c r="N5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>0</v>
+      <c r="D6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="F6" s="2" t="b">
         <v>0</v>
@@ -1238,10 +1408,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="2" t="b">
         <v>0</v>
@@ -1250,33 +1420,36 @@
         <v>0</v>
       </c>
       <c r="N6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="2" t="b">
-        <v>1</v>
+      <c r="D7" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="F7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>0</v>
@@ -1288,10 +1461,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="2" t="b">
         <v>0</v>
@@ -1300,33 +1473,34 @@
         <v>0</v>
       </c>
       <c r="N7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="2" t="b">
-        <v>1</v>
+      <c r="D8" s="8"/>
+      <c r="E8" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="F8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="b">
         <v>0</v>
@@ -1350,30 +1524,33 @@
         <v>0</v>
       </c>
       <c r="N8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" s="2" t="b">
-        <v>0</v>
+      <c r="D9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="F9" s="2" t="b">
         <v>0</v>
@@ -1388,10 +1565,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="2" t="b">
         <v>0</v>
@@ -1400,30 +1577,33 @@
         <v>0</v>
       </c>
       <c r="N9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="2" t="b">
-        <v>0</v>
+      <c r="D10" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="F10" s="2" t="b">
         <v>0</v>
@@ -1438,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="2" t="b">
         <v>0</v>
@@ -1450,48 +1630,51 @@
         <v>0</v>
       </c>
       <c r="N10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="2" t="b">
-        <v>0</v>
+      <c r="D11" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="F11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="2" t="b">
         <v>0</v>
@@ -1500,30 +1683,33 @@
         <v>0</v>
       </c>
       <c r="N11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="2" t="b">
-        <v>0</v>
+      <c r="D12" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="F12" s="2" t="b">
         <v>0</v>
@@ -1538,10 +1724,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2" t="b">
         <v>0</v>
@@ -1553,30 +1739,30 @@
         <v>0</v>
       </c>
       <c r="O12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
+      <c r="E13" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="F13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>0</v>
@@ -1603,51 +1789,54 @@
         <v>0</v>
       </c>
       <c r="O13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E14" s="2" t="b">
-        <v>1</v>
+      <c r="D14" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>173</v>
       </c>
       <c r="F14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2" t="b">
         <v>0</v>
@@ -1658,25 +1847,26 @@
       <c r="P14" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="D15" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="17"/>
       <c r="F15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>0</v>
@@ -1694,10 +1884,10 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="2" t="b">
         <v>0</v>
@@ -1706,24 +1896,27 @@
         <v>0</v>
       </c>
       <c r="P15" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>0</v>
+      <c r="D16" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="F16" s="2" t="b">
         <v>0</v>
@@ -1741,13 +1934,13 @@
         <v>0</v>
       </c>
       <c r="K16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="2" t="b">
         <v>0</v>
@@ -1756,24 +1949,27 @@
         <v>0</v>
       </c>
       <c r="P16" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <v>0</v>
+      <c r="D17" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="F17" s="2" t="b">
         <v>0</v>
@@ -1782,10 +1978,10 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="2" t="b">
         <v>0</v>
@@ -1794,10 +1990,10 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="2" t="b">
         <v>0</v>
@@ -1806,24 +2002,27 @@
         <v>0</v>
       </c>
       <c r="P17" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E18" s="2" t="b">
-        <v>0</v>
+      <c r="D18" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="F18" s="2" t="b">
         <v>0</v>
@@ -1841,13 +2040,13 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2" t="b">
         <v>0</v>
@@ -1856,24 +2055,27 @@
         <v>0</v>
       </c>
       <c r="P18" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <v>0</v>
+      <c r="D19" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="F19" s="2" t="b">
         <v>0</v>
@@ -1891,13 +2093,13 @@
         <v>0</v>
       </c>
       <c r="K19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="2" t="b">
         <v>0</v>
@@ -1906,27 +2108,30 @@
         <v>0</v>
       </c>
       <c r="P19" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20" s="2" t="b">
-        <v>1</v>
+      <c r="D20" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="F20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2" t="b">
         <v>0</v>
@@ -1944,10 +2149,10 @@
         <v>0</v>
       </c>
       <c r="L20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="2" t="b">
         <v>0</v>
@@ -1958,22 +2163,25 @@
       <c r="P20" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q20" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" s="2" t="b">
-        <v>0</v>
+      <c r="D21" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>183</v>
       </c>
       <c r="F21" s="2" t="b">
         <v>0</v>
@@ -1985,19 +2193,19 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="2" t="b">
         <v>0</v>
@@ -2008,22 +2216,25 @@
       <c r="P21" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q21" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E22" s="2" t="b">
-        <v>0</v>
+      <c r="D22" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="F22" s="2" t="b">
         <v>0</v>
@@ -2041,13 +2252,13 @@
         <v>0</v>
       </c>
       <c r="K22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="2" t="b">
         <v>0</v>
@@ -2056,24 +2267,27 @@
         <v>0</v>
       </c>
       <c r="P22" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
       <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="2" t="b">
-        <v>0</v>
+      <c r="D23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="F23" s="2" t="b">
         <v>0</v>
@@ -2085,19 +2299,19 @@
         <v>0</v>
       </c>
       <c r="I23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="2" t="b">
         <v>1</v>
       </c>
       <c r="K23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="2" t="b">
         <v>0</v>
@@ -2108,22 +2322,25 @@
       <c r="P23" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q23" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="2" t="b">
-        <v>0</v>
+      <c r="D24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>184</v>
       </c>
       <c r="F24" s="2" t="b">
         <v>0</v>
@@ -2132,10 +2349,10 @@
         <v>0</v>
       </c>
       <c r="H24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="2" t="b">
         <v>0</v>
@@ -2144,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2" t="b">
         <v>0</v>
@@ -2158,28 +2375,31 @@
       <c r="P24" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E25" s="2" t="b">
-        <v>0</v>
+      <c r="D25" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="F25" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="2" t="b">
         <v>0</v>
@@ -2203,33 +2423,36 @@
         <v>0</v>
       </c>
       <c r="O25" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q25" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>61</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E26" s="2" t="b">
-        <v>0</v>
+      <c r="D26" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="F26" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2" t="b">
         <v>0</v>
@@ -2244,10 +2467,10 @@
         <v>0</v>
       </c>
       <c r="L26" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="2" t="b">
         <v>0</v>
@@ -2258,22 +2481,25 @@
       <c r="P26" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q26" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>0</v>
+      <c r="D27" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="F27" s="2" t="b">
         <v>0</v>
@@ -2285,19 +2511,19 @@
         <v>0</v>
       </c>
       <c r="I27" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L27" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="2" t="b">
         <v>0</v>
@@ -2308,22 +2534,25 @@
       <c r="P27" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q27" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>65</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E28" s="2" t="b">
-        <v>0</v>
+      <c r="D28" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="F28" s="2" t="b">
         <v>0</v>
@@ -2341,13 +2570,13 @@
         <v>0</v>
       </c>
       <c r="K28" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M28" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="2" t="b">
         <v>0</v>
@@ -2356,24 +2585,27 @@
         <v>0</v>
       </c>
       <c r="P28" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>67</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>0</v>
+      <c r="D29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="F29" s="2" t="b">
         <v>0</v>
@@ -2385,19 +2617,19 @@
         <v>0</v>
       </c>
       <c r="I29" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L29" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="2" t="b">
         <v>0</v>
@@ -2408,46 +2640,49 @@
       <c r="P29" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q29" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>68</v>
       </c>
       <c r="B30" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="2" t="b">
-        <v>0</v>
+      <c r="D30" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="F30" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I30" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L30" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="2" t="b">
         <v>0</v>
@@ -2458,22 +2693,25 @@
       <c r="P30" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
       <c r="B31" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>0</v>
+      <c r="D31" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="F31" s="2" t="b">
         <v>0</v>
@@ -2491,13 +2729,13 @@
         <v>0</v>
       </c>
       <c r="K31" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M31" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="2" t="b">
         <v>0</v>
@@ -2506,24 +2744,27 @@
         <v>0</v>
       </c>
       <c r="P31" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
       <c r="B32" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" s="2" t="b">
-        <v>0</v>
+      <c r="D32" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="F32" s="2" t="b">
         <v>0</v>
@@ -2538,10 +2779,10 @@
         <v>0</v>
       </c>
       <c r="J32" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" s="2" t="b">
         <v>0</v>
@@ -2553,30 +2794,33 @@
         <v>0</v>
       </c>
       <c r="O32" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="2" t="b">
-        <v>1</v>
+      <c r="D33" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="F33" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="2" t="b">
         <v>0</v>
@@ -2594,10 +2838,10 @@
         <v>0</v>
       </c>
       <c r="L33" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="2" t="b">
         <v>0</v>
@@ -2606,27 +2850,30 @@
         <v>0</v>
       </c>
       <c r="P33" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>76</v>
       </c>
       <c r="B34" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>1</v>
+      <c r="D34" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>192</v>
       </c>
       <c r="F34" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="2" t="b">
         <v>0</v>
@@ -2644,10 +2891,10 @@
         <v>0</v>
       </c>
       <c r="L34" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="2" t="b">
         <v>0</v>
@@ -2656,24 +2903,27 @@
         <v>0</v>
       </c>
       <c r="P34" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>78</v>
       </c>
       <c r="B35" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="2" t="b">
-        <v>0</v>
+      <c r="D35" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="F35" s="2" t="b">
         <v>0</v>
@@ -2691,13 +2941,13 @@
         <v>0</v>
       </c>
       <c r="K35" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M35" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="2" t="b">
         <v>0</v>
@@ -2706,24 +2956,27 @@
         <v>0</v>
       </c>
       <c r="P35" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>80</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" s="2" t="b">
-        <v>0</v>
+      <c r="D36" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="F36" s="2" t="b">
         <v>0</v>
@@ -2732,10 +2985,10 @@
         <v>0</v>
       </c>
       <c r="H36" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="2" t="b">
         <v>0</v>
@@ -2744,10 +2997,10 @@
         <v>0</v>
       </c>
       <c r="L36" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" s="2" t="b">
         <v>0</v>
@@ -2758,22 +3011,25 @@
       <c r="P36" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q36" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>81</v>
       </c>
       <c r="B37" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" s="2" t="b">
-        <v>0</v>
+      <c r="D37" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="F37" s="2" t="b">
         <v>0</v>
@@ -2785,19 +3041,19 @@
         <v>0</v>
       </c>
       <c r="I37" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L37" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37" s="2" t="b">
         <v>0</v>
@@ -2808,22 +3064,25 @@
       <c r="P37" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q37" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
       <c r="B38" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>0</v>
+      <c r="D38" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>183</v>
       </c>
       <c r="F38" s="2" t="b">
         <v>0</v>
@@ -2832,10 +3091,10 @@
         <v>0</v>
       </c>
       <c r="H38" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="2" t="b">
         <v>0</v>
@@ -2844,10 +3103,10 @@
         <v>0</v>
       </c>
       <c r="L38" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38" s="2" t="b">
         <v>0</v>
@@ -2858,22 +3117,25 @@
       <c r="P38" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q38" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>85</v>
       </c>
       <c r="B39" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="2" t="b">
-        <v>0</v>
+      <c r="D39" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="F39" s="2" t="b">
         <v>0</v>
@@ -2882,10 +3144,10 @@
         <v>0</v>
       </c>
       <c r="H39" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="2" t="b">
         <v>0</v>
@@ -2894,10 +3156,10 @@
         <v>0</v>
       </c>
       <c r="L39" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="2" t="b">
         <v>0</v>
@@ -2906,24 +3168,27 @@
         <v>0</v>
       </c>
       <c r="P39" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="2" t="b">
-        <v>0</v>
+      <c r="D40" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="F40" s="2" t="b">
         <v>0</v>
@@ -2932,10 +3197,10 @@
         <v>0</v>
       </c>
       <c r="H40" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="2" t="b">
         <v>0</v>
@@ -2944,10 +3209,10 @@
         <v>0</v>
       </c>
       <c r="L40" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" s="2" t="b">
         <v>0</v>
@@ -2956,24 +3221,27 @@
         <v>0</v>
       </c>
       <c r="P40" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>89</v>
       </c>
       <c r="B41" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E41" s="2" t="b">
-        <v>0</v>
+      <c r="D41" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F41" s="2" t="b">
         <v>0</v>
@@ -2982,10 +3250,10 @@
         <v>0</v>
       </c>
       <c r="H41" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="2" t="b">
         <v>0</v>
@@ -2994,10 +3262,10 @@
         <v>0</v>
       </c>
       <c r="L41" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N41" s="2" t="b">
         <v>0</v>
@@ -3006,30 +3274,33 @@
         <v>0</v>
       </c>
       <c r="P41" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>0</v>
+      <c r="D42" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="F42" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="2" t="b">
         <v>0</v>
@@ -3044,10 +3315,10 @@
         <v>0</v>
       </c>
       <c r="L42" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N42" s="2" t="b">
         <v>0</v>
@@ -3058,28 +3329,31 @@
       <c r="P42" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q42" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>93</v>
       </c>
       <c r="B43" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>0</v>
+      <c r="D43" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>195</v>
       </c>
       <c r="F43" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="2" t="b">
         <v>0</v>
@@ -3097,36 +3371,39 @@
         <v>0</v>
       </c>
       <c r="M43" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P43" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>95</v>
       </c>
       <c r="B44" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>1</v>
+      <c r="D44" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="F44" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="2" t="b">
         <v>0</v>
@@ -3147,10 +3424,10 @@
         <v>0</v>
       </c>
       <c r="M44" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" s="2" t="b">
         <v>0</v>
@@ -3158,22 +3435,25 @@
       <c r="P44" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q44" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>97</v>
       </c>
       <c r="B45" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" s="2" t="b">
-        <v>0</v>
+      <c r="D45" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="F45" s="2" t="b">
         <v>0</v>
@@ -3191,16 +3471,16 @@
         <v>0</v>
       </c>
       <c r="K45" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M45" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O45" s="2" t="b">
         <v>0</v>
@@ -3208,31 +3488,34 @@
       <c r="P45" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q45" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>99</v>
       </c>
       <c r="B46" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
+      <c r="D46" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>193</v>
       </c>
       <c r="F46" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G46" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" s="2" t="b">
         <v>0</v>
@@ -3247,10 +3530,10 @@
         <v>0</v>
       </c>
       <c r="M46" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O46" s="2" t="b">
         <v>0</v>
@@ -3258,25 +3541,28 @@
       <c r="P46" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q46" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>101</v>
       </c>
       <c r="B47" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E47" s="2" t="b">
-        <v>1</v>
+      <c r="D47" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="F47" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="2" t="b">
         <v>0</v>
@@ -3297,33 +3583,36 @@
         <v>0</v>
       </c>
       <c r="M47" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P47" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>103</v>
       </c>
       <c r="B48" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <v>0</v>
+      <c r="D48" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>190</v>
       </c>
       <c r="F48" s="2" t="b">
         <v>0</v>
@@ -3347,39 +3636,40 @@
         <v>0</v>
       </c>
       <c r="M48" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N48" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P48" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>105</v>
       </c>
       <c r="B49" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="D49" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="20"/>
       <c r="F49" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="2" t="b">
         <v>0</v>
@@ -3397,39 +3687,42 @@
         <v>0</v>
       </c>
       <c r="M49" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N49" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P49" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>107</v>
       </c>
       <c r="B50" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" s="2" t="b">
-        <v>0</v>
+      <c r="D50" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>196</v>
       </c>
       <c r="F50" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="2" t="b">
         <v>0</v>
@@ -3447,10 +3740,10 @@
         <v>0</v>
       </c>
       <c r="M50" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N50" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50" s="2" t="b">
         <v>0</v>
@@ -3458,22 +3751,25 @@
       <c r="P50" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q50" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>109</v>
       </c>
       <c r="B51" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="2" t="b">
-        <v>0</v>
+      <c r="D51" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="F51" s="2" t="b">
         <v>0</v>
@@ -3491,42 +3787,45 @@
         <v>0</v>
       </c>
       <c r="K51" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P51" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>111</v>
       </c>
       <c r="B52" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
+      <c r="D52" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="F52" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="2" t="b">
         <v>0</v>
@@ -3547,36 +3846,39 @@
         <v>0</v>
       </c>
       <c r="M52" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N52" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P52" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
       <c r="B53" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E53" s="2" t="b">
-        <v>1</v>
+      <c r="D53" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>172</v>
       </c>
       <c r="F53" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="2" t="b">
         <v>0</v>
@@ -3597,33 +3899,36 @@
         <v>0</v>
       </c>
       <c r="M53" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N53" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P53" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>115</v>
       </c>
       <c r="B54" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E54" s="2" t="b">
-        <v>0</v>
+      <c r="D54" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="F54" s="2" t="b">
         <v>0</v>
@@ -3647,10 +3952,10 @@
         <v>0</v>
       </c>
       <c r="M54" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N54" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O54" s="2" t="b">
         <v>0</v>
@@ -3658,31 +3963,34 @@
       <c r="P54" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q54" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>117</v>
       </c>
       <c r="B55" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>0</v>
+      <c r="D55" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="F55" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G55" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="2" t="b">
         <v>0</v>
@@ -3697,10 +4005,10 @@
         <v>0</v>
       </c>
       <c r="M55" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O55" s="2" t="b">
         <v>0</v>
@@ -3708,31 +4016,34 @@
       <c r="P55" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q55" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>119</v>
       </c>
       <c r="B56" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E56" s="2" t="b">
-        <v>0</v>
+      <c r="D56" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>182</v>
       </c>
       <c r="F56" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G56" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="2" t="b">
         <v>0</v>
@@ -3747,39 +4058,42 @@
         <v>0</v>
       </c>
       <c r="M56" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P56" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>121</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E57" s="2" t="b">
-        <v>0</v>
+      <c r="D57" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>196</v>
       </c>
       <c r="F57" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="2" t="b">
         <v>0</v>
@@ -3797,10 +4111,10 @@
         <v>0</v>
       </c>
       <c r="M57" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N57" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57" s="2" t="b">
         <v>0</v>
@@ -3808,28 +4122,31 @@
       <c r="P57" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q57" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>122</v>
       </c>
       <c r="B58" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>0</v>
+      <c r="D58" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>196</v>
       </c>
       <c r="F58" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="2" t="b">
         <v>0</v>
@@ -3847,36 +4164,39 @@
         <v>0</v>
       </c>
       <c r="M58" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N58" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P58" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>124</v>
       </c>
       <c r="B59" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D59" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E59" s="2" t="b">
-        <v>1</v>
+      <c r="D59" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>196</v>
       </c>
       <c r="F59" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="2" t="b">
         <v>0</v>
@@ -3897,10 +4217,10 @@
         <v>0</v>
       </c>
       <c r="M59" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N59" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O59" s="2" t="b">
         <v>0</v>
@@ -3908,22 +4228,25 @@
       <c r="P59" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q59" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>126</v>
       </c>
       <c r="B60" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E60" s="2" t="b">
-        <v>0</v>
+      <c r="D60" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>190</v>
       </c>
       <c r="F60" s="2" t="b">
         <v>0</v>
@@ -3947,33 +4270,36 @@
         <v>0</v>
       </c>
       <c r="M60" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N60" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P60" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>128</v>
       </c>
       <c r="B61" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E61" s="2" t="b">
-        <v>0</v>
+      <c r="D61" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>190</v>
       </c>
       <c r="F61" s="2" t="b">
         <v>0</v>
@@ -3997,33 +4323,36 @@
         <v>0</v>
       </c>
       <c r="M61" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N61" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P61" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>130</v>
       </c>
       <c r="B62" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
+      <c r="D62" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>182</v>
       </c>
       <c r="F62" s="2" t="b">
         <v>0</v>
@@ -4032,10 +4361,10 @@
         <v>0</v>
       </c>
       <c r="H62" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="2" t="b">
         <v>0</v>
@@ -4047,33 +4376,36 @@
         <v>0</v>
       </c>
       <c r="M62" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N62" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P62" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>132</v>
       </c>
       <c r="B63" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>0</v>
+      <c r="D63" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E63" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="F63" s="2" t="b">
         <v>0</v>
@@ -4082,10 +4414,10 @@
         <v>0</v>
       </c>
       <c r="H63" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="2" t="b">
         <v>0</v>
@@ -4097,39 +4429,42 @@
         <v>0</v>
       </c>
       <c r="M63" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N63" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O63" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P63" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>134</v>
       </c>
       <c r="B64" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E64" s="2" t="b">
-        <v>0</v>
+      <c r="D64" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>186</v>
       </c>
       <c r="F64" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="2" t="b">
         <v>0</v>
@@ -4147,39 +4482,42 @@
         <v>0</v>
       </c>
       <c r="M64" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N64" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P64" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>136</v>
       </c>
       <c r="B65" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D65" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
+      <c r="D65" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="F65" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="2" t="b">
         <v>0</v>
@@ -4197,36 +4535,39 @@
         <v>0</v>
       </c>
       <c r="M65" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N65" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P65" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>138</v>
       </c>
       <c r="B66" t="s">
         <v>139</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>1</v>
+      <c r="D66" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>176</v>
       </c>
       <c r="F66" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="2" t="b">
         <v>0</v>
@@ -4247,10 +4588,10 @@
         <v>0</v>
       </c>
       <c r="M66" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N66" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O66" s="2" t="b">
         <v>0</v>
@@ -4258,28 +4599,31 @@
       <c r="P66" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q66" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>140</v>
       </c>
       <c r="B67" t="s">
         <v>141</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
+      <c r="D67" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="F67" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="2" t="b">
         <v>0</v>
@@ -4297,36 +4641,39 @@
         <v>0</v>
       </c>
       <c r="M67" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N67" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P67" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>142</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D68" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>1</v>
+      <c r="D68" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>186</v>
       </c>
       <c r="F68" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="2" t="b">
         <v>0</v>
@@ -4347,10 +4694,10 @@
         <v>0</v>
       </c>
       <c r="M68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N68" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O68" s="2" t="b">
         <v>0</v>
@@ -4358,28 +4705,31 @@
       <c r="P68" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q68" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>143</v>
       </c>
       <c r="B69" t="s">
         <v>144</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
+      <c r="D69" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="F69" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="2" t="b">
         <v>0</v>
@@ -4397,15 +4747,18 @@
         <v>0</v>
       </c>
       <c r="M69" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>